<commit_message>
one hot encoder notes
</commit_message>
<xml_diff>
--- a/regression.xlsx
+++ b/regression.xlsx
@@ -522,11 +522,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="806535637"/>
-        <c:axId val="202964885"/>
+        <c:axId val="2036578250"/>
+        <c:axId val="1082815964"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="806535637"/>
+        <c:axId val="2036578250"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -601,10 +601,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202964885"/>
+        <c:crossAx val="1082815964"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="202964885"/>
+        <c:axId val="1082815964"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -679,7 +679,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="806535637"/>
+        <c:crossAx val="2036578250"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -816,11 +816,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1324924909"/>
-        <c:axId val="1779102565"/>
+        <c:axId val="1372370848"/>
+        <c:axId val="1337738354"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1324924909"/>
+        <c:axId val="1372370848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -895,10 +895,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1779102565"/>
+        <c:crossAx val="1337738354"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1779102565"/>
+        <c:axId val="1337738354"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -973,7 +973,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1324924909"/>
+        <c:crossAx val="1372370848"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1076,11 +1076,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="111082466"/>
-        <c:axId val="1806025914"/>
+        <c:axId val="2099700425"/>
+        <c:axId val="854997396"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="111082466"/>
+        <c:axId val="2099700425"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1155,10 +1155,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1806025914"/>
+        <c:crossAx val="854997396"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1806025914"/>
+        <c:axId val="854997396"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1233,7 +1233,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="111082466"/>
+        <c:crossAx val="2099700425"/>
       </c:valAx>
     </c:plotArea>
   </c:chart>
@@ -1241,6 +1241,285 @@
 </file>
 
 <file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>estimate vs. # of bedrooms</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'high bed'!$F$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:name>Trendline for price</c:name>
+            <c:spPr>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'high bed'!$B$2:$B$21</c:f>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'high bed'!$F$2:$F$21</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1963411296"/>
+        <c:axId val="518419543"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1963411296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t># of bedrooms</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="518419543"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="518419543"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>estimate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1963411296"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:title>
@@ -1318,11 +1597,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1424224636"/>
-        <c:axId val="2064496688"/>
+        <c:axId val="507373563"/>
+        <c:axId val="263783608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1424224636"/>
+        <c:axId val="507373563"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1397,10 +1676,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2064496688"/>
+        <c:crossAx val="263783608"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2064496688"/>
+        <c:axId val="263783608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1475,14 +1754,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1424224636"/>
+        <c:crossAx val="507373563"/>
       </c:valAx>
     </c:plotArea>
   </c:chart>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:title>
@@ -1560,11 +1839,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1547615270"/>
-        <c:axId val="1211185261"/>
+        <c:axId val="381190616"/>
+        <c:axId val="1614998093"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1547615270"/>
+        <c:axId val="381190616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1639,10 +1918,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1211185261"/>
+        <c:crossAx val="1614998093"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1211185261"/>
+        <c:axId val="1614998093"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1717,14 +1996,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1547615270"/>
+        <c:crossAx val="381190616"/>
       </c:valAx>
     </c:plotArea>
   </c:chart>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:title>
@@ -1835,11 +2114,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="32750570"/>
-        <c:axId val="1996054661"/>
+        <c:axId val="1181953615"/>
+        <c:axId val="1417754328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="32750570"/>
+        <c:axId val="1181953615"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1914,10 +2193,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1996054661"/>
+        <c:crossAx val="1417754328"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1996054661"/>
+        <c:axId val="1417754328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1992,7 +2271,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32750570"/>
+        <c:crossAx val="1181953615"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2017,7 +2296,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:title>
@@ -2128,11 +2407,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="723707218"/>
-        <c:axId val="2011000172"/>
+        <c:axId val="886817330"/>
+        <c:axId val="336438065"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="723707218"/>
+        <c:axId val="886817330"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2207,10 +2486,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2011000172"/>
+        <c:crossAx val="336438065"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2011000172"/>
+        <c:axId val="336438065"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2285,7 +2564,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="723707218"/>
+        <c:crossAx val="886817330"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2310,7 +2589,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:title>
@@ -2388,11 +2667,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="454139171"/>
-        <c:axId val="351316753"/>
+        <c:axId val="298133733"/>
+        <c:axId val="389956687"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="454139171"/>
+        <c:axId val="298133733"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2467,10 +2746,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="351316753"/>
+        <c:crossAx val="389956687"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="351316753"/>
+        <c:axId val="389956687"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2545,14 +2824,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="454139171"/>
+        <c:crossAx val="298133733"/>
       </c:valAx>
     </c:plotArea>
   </c:chart>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:title>
@@ -2630,11 +2909,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1603497508"/>
-        <c:axId val="625036024"/>
+        <c:axId val="64762535"/>
+        <c:axId val="1994931891"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1603497508"/>
+        <c:axId val="64762535"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2709,10 +2988,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="625036024"/>
+        <c:crossAx val="1994931891"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="625036024"/>
+        <c:axId val="1994931891"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2787,14 +3066,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1603497508"/>
+        <c:crossAx val="64762535"/>
       </c:valAx>
     </c:plotArea>
   </c:chart>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:title>
@@ -2872,11 +3151,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1158818055"/>
-        <c:axId val="1040616829"/>
+        <c:axId val="746055371"/>
+        <c:axId val="1327392189"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1158818055"/>
+        <c:axId val="746055371"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2951,10 +3230,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1040616829"/>
+        <c:crossAx val="1327392189"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1040616829"/>
+        <c:axId val="1327392189"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3029,14 +3308,252 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1158818055"/>
+        <c:crossAx val="746055371"/>
       </c:valAx>
     </c:plotArea>
   </c:chart>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>correlation!$B$16</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>correlation!$A$17:$A$21</c:f>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>correlation!$B$17:$B$21</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="532107797"/>
+        <c:axId val="1379414942"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="532107797"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1379414942"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1379414942"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="532107797"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:title>
@@ -3147,11 +3664,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1776134651"/>
-        <c:axId val="2045874884"/>
+        <c:axId val="225906736"/>
+        <c:axId val="475032557"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1776134651"/>
+        <c:axId val="225906736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3226,10 +3743,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2045874884"/>
+        <c:crossAx val="475032557"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2045874884"/>
+        <c:axId val="475032557"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3304,7 +3821,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1776134651"/>
+        <c:crossAx val="225906736"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3329,245 +3846,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>correlation!$B$16</c:f>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="7"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln cmpd="sng">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>correlation!$A$17:$A$21</c:f>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>correlation!$B$17:$B$21</c:f>
-              <c:numCache/>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1974341034"/>
-        <c:axId val="1985624950"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1974341034"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="B7B7B7"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="CCCCCC">
-                  <a:alpha val="0"/>
-                </a:srgbClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr lvl="0">
-                  <a:defRPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t/>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1985624950"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="1985624950"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="B7B7B7"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="CCCCCC">
-                  <a:alpha val="0"/>
-                </a:srgbClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr lvl="0">
-                  <a:defRPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t/>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1974341034"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0">
-            <a:defRPr b="0">
-              <a:solidFill>
-                <a:srgbClr val="1A1A1A"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:title>
@@ -3678,11 +3957,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="535832846"/>
-        <c:axId val="336301342"/>
+        <c:axId val="1013514588"/>
+        <c:axId val="1843307389"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="535832846"/>
+        <c:axId val="1013514588"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3757,10 +4036,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="336301342"/>
+        <c:crossAx val="1843307389"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="336301342"/>
+        <c:axId val="1843307389"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3835,7 +4114,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="535832846"/>
+        <c:crossAx val="1013514588"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3860,7 +4139,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:title>
@@ -3938,11 +4217,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1591222758"/>
-        <c:axId val="2084446916"/>
+        <c:axId val="1544176753"/>
+        <c:axId val="863910905"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1591222758"/>
+        <c:axId val="1544176753"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4017,10 +4296,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2084446916"/>
+        <c:crossAx val="863910905"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2084446916"/>
+        <c:axId val="863910905"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4095,14 +4374,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1591222758"/>
+        <c:crossAx val="1544176753"/>
       </c:valAx>
     </c:plotArea>
   </c:chart>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:title>
@@ -4180,11 +4459,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1029541276"/>
-        <c:axId val="303097828"/>
+        <c:axId val="740100639"/>
+        <c:axId val="328157010"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1029541276"/>
+        <c:axId val="740100639"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4259,10 +4538,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="303097828"/>
+        <c:crossAx val="328157010"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="303097828"/>
+        <c:axId val="328157010"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4337,14 +4616,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1029541276"/>
+        <c:crossAx val="740100639"/>
       </c:valAx>
     </c:plotArea>
   </c:chart>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:title>
@@ -4422,11 +4701,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="323329979"/>
-        <c:axId val="1043344529"/>
+        <c:axId val="445835599"/>
+        <c:axId val="129546514"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="323329979"/>
+        <c:axId val="445835599"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4501,10 +4780,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1043344529"/>
+        <c:crossAx val="129546514"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1043344529"/>
+        <c:axId val="129546514"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4579,14 +4858,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="323329979"/>
+        <c:crossAx val="445835599"/>
       </c:valAx>
     </c:plotArea>
   </c:chart>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:title>
@@ -4697,11 +4976,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1348875814"/>
-        <c:axId val="1020839696"/>
+        <c:axId val="1849751424"/>
+        <c:axId val="171604349"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1348875814"/>
+        <c:axId val="1849751424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4776,10 +5055,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1020839696"/>
+        <c:crossAx val="171604349"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1020839696"/>
+        <c:axId val="171604349"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4854,7 +5133,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1348875814"/>
+        <c:crossAx val="1849751424"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -4879,7 +5158,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:title>
@@ -4990,11 +5269,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="61738722"/>
-        <c:axId val="1516751021"/>
+        <c:axId val="1442098031"/>
+        <c:axId val="548446979"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61738722"/>
+        <c:axId val="1442098031"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5069,10 +5348,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1516751021"/>
+        <c:crossAx val="548446979"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1516751021"/>
+        <c:axId val="548446979"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5147,7 +5426,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61738722"/>
+        <c:crossAx val="1442098031"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -5172,7 +5451,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:title>
@@ -5250,11 +5529,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="141463002"/>
-        <c:axId val="1010731637"/>
+        <c:axId val="1141271666"/>
+        <c:axId val="1643401002"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="141463002"/>
+        <c:axId val="1141271666"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5329,10 +5608,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1010731637"/>
+        <c:crossAx val="1643401002"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1010731637"/>
+        <c:axId val="1643401002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5407,7 +5686,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="141463002"/>
+        <c:crossAx val="1141271666"/>
       </c:valAx>
     </c:plotArea>
   </c:chart>
@@ -5469,11 +5748,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1956046179"/>
-        <c:axId val="1905232742"/>
+        <c:axId val="439620308"/>
+        <c:axId val="1737168153"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1956046179"/>
+        <c:axId val="439620308"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5548,10 +5827,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1905232742"/>
+        <c:crossAx val="1737168153"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1905232742"/>
+        <c:axId val="1737168153"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5626,7 +5905,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1956046179"/>
+        <c:crossAx val="439620308"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -5748,11 +6027,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="705501373"/>
-        <c:axId val="931434878"/>
+        <c:axId val="1679114054"/>
+        <c:axId val="571695200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="705501373"/>
+        <c:axId val="1679114054"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5827,10 +6106,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="931434878"/>
+        <c:crossAx val="571695200"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="931434878"/>
+        <c:axId val="571695200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5905,7 +6184,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="705501373"/>
+        <c:crossAx val="1679114054"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -6027,11 +6306,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1023496352"/>
-        <c:axId val="1196497292"/>
+        <c:axId val="1987670909"/>
+        <c:axId val="683616254"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1023496352"/>
+        <c:axId val="1987670909"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6106,10 +6385,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1196497292"/>
+        <c:crossAx val="683616254"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1196497292"/>
+        <c:axId val="683616254"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6184,7 +6463,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1023496352"/>
+        <c:crossAx val="1987670909"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -6306,11 +6585,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="972019475"/>
-        <c:axId val="1729421499"/>
+        <c:axId val="844111030"/>
+        <c:axId val="1466606199"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="972019475"/>
+        <c:axId val="844111030"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6385,10 +6664,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1729421499"/>
+        <c:crossAx val="1466606199"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1729421499"/>
+        <c:axId val="1466606199"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6463,7 +6742,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="972019475"/>
+        <c:crossAx val="844111030"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -6567,11 +6846,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2108400957"/>
-        <c:axId val="402233528"/>
+        <c:axId val="1900431882"/>
+        <c:axId val="1351044822"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2108400957"/>
+        <c:axId val="1900431882"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6646,10 +6925,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="402233528"/>
+        <c:crossAx val="1351044822"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="402233528"/>
+        <c:axId val="1351044822"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6724,7 +7003,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2108400957"/>
+        <c:crossAx val="1900431882"/>
       </c:valAx>
     </c:plotArea>
   </c:chart>
@@ -6809,11 +7088,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1952282258"/>
-        <c:axId val="1053363792"/>
+        <c:axId val="203205392"/>
+        <c:axId val="1005071663"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1952282258"/>
+        <c:axId val="203205392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6888,10 +7167,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1053363792"/>
+        <c:crossAx val="1005071663"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1053363792"/>
+        <c:axId val="1005071663"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6966,7 +7245,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1952282258"/>
+        <c:crossAx val="203205392"/>
       </c:valAx>
     </c:plotArea>
   </c:chart>
@@ -7084,11 +7363,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1077017063"/>
-        <c:axId val="1371497210"/>
+        <c:axId val="1813314160"/>
+        <c:axId val="1319596249"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1077017063"/>
+        <c:axId val="1813314160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7163,10 +7442,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1371497210"/>
+        <c:crossAx val="1319596249"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1371497210"/>
+        <c:axId val="1319596249"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7241,7 +7520,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1077017063"/>
+        <c:crossAx val="1813314160"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -7552,6 +7831,31 @@
     </xdr:graphicFrame>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3533775"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 12" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7567,7 +7871,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="12" name="Chart 12"/>
+        <xdr:cNvPr id="13" name="Chart 13"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7592,7 +7896,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="13" name="Chart 13"/>
+        <xdr:cNvPr id="14" name="Chart 14"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7617,7 +7921,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="14" name="Chart 14"/>
+        <xdr:cNvPr id="15" name="Chart 15"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7642,7 +7946,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="15" name="Chart 15"/>
+        <xdr:cNvPr id="16" name="Chart 16"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7667,7 +7971,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="16" name="Chart 16"/>
+        <xdr:cNvPr id="17" name="Chart 17"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7697,7 +8001,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="17" name="Chart 17"/>
+        <xdr:cNvPr id="18" name="Chart 18"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7722,7 +8026,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="18" name="Chart 18"/>
+        <xdr:cNvPr id="19" name="Chart 19"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7747,7 +8051,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="19" name="Chart 19"/>
+        <xdr:cNvPr id="20" name="Chart 20"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7772,7 +8076,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="20" name="Chart 20"/>
+        <xdr:cNvPr id="21" name="Chart 21"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7797,7 +8101,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="21" name="Chart 21"/>
+        <xdr:cNvPr id="22" name="Chart 22"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7827,7 +8131,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="22" name="Chart 22"/>
+        <xdr:cNvPr id="23" name="Chart 23"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7852,7 +8156,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="23" name="Chart 23"/>
+        <xdr:cNvPr id="24" name="Chart 24"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7877,7 +8181,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="24" name="Chart 24"/>
+        <xdr:cNvPr id="25" name="Chart 25"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7902,7 +8206,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="25" name="Chart 25"/>
+        <xdr:cNvPr id="26" name="Chart 26"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7927,7 +8231,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="26" name="Chart 26"/>
+        <xdr:cNvPr id="27" name="Chart 27"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>

</xml_diff>